<commit_message>
title and authors in supplementary materials
</commit_message>
<xml_diff>
--- a/results/supplementary/FEEspinosadelAlbaST1.xlsx
+++ b/results/supplementary/FEEspinosadelAlbaST1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioviedo-my.sharepoint.com/personal/espinosaclara_uniovi_es/Documents/IMIB/Softwares/GitHub/Hidro_thermal_experiments/results/supplementary/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioviedo-my.sharepoint.com/personal/espinosaclara_uniovi_es/Documents/IMIB/Softwares/GitHub/Dianthus_PEG/results/supplementary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4D1D1112-CE95-4D9C-926D-F18C2375F41A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="8_{4D1D1112-CE95-4D9C-926D-F18C2375F41A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{26F74EDC-888B-4BFB-B3D3-DB568F3CCBE9}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="570" windowWidth="14385" windowHeight="14400" xr2:uid="{068E1733-3400-45CC-8D0E-5CDF90EB1089}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{068E1733-3400-45CC-8D0E-5CDF90EB1089}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>Site</t>
   </si>
@@ -126,6 +126,12 @@
   </si>
   <si>
     <t>C20</t>
+  </si>
+  <si>
+    <t>Supporting Table 1: Subpopulations bioclimatic indices. Bio1 = annual mean temperature; bio2 = mean diurnal range, i.e., the mean of the monthly differences between maximum and minimum temperatures; bio7 = temperature annual range; i.e. the difference between the maximum temperature of the warmest month and the minimum temperature of the coldest month; snow = the number of days of snow cover, when the soil temperature is around 0 °C, calculated for the period in which the maximum temperature was &lt; 0.5 °C and the minimum temperature was &gt; -0.5 °C;  FDD = freezing degree days, i.e. the sum of daily mean temperatures for days in which the mean temperature was below 0 °C (Choler, 2018); and GDD = growing degree days, i.e. the sum of daily mean temperatures for days in which the soil mean temperature at five cm deep was above 5 °C (Körner, 2021). For easier interpretation of FDD, we transformed the values from negative to positive.</t>
+  </si>
+  <si>
+    <t>Functional intraspecific variation in the base water potential for seed germination along soil microclimatic gradients. Espinosa del Alba, C., Cruz-Tejada, D., Jiménez-Alfaro, B., and E. Fernández-Pascual. (2025). Functional Ecology.</t>
   </si>
 </sst>
 </file>
@@ -161,8 +167,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -178,6 +187,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -497,142 +510,128 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F05EBED7-2849-4B63-A125-84B437CD3D0B}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A20" sqref="A20:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
+    <row r="1" spans="1:8" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2">
-        <v>6.6774736802061101</v>
-      </c>
-      <c r="D2">
-        <v>6.0704386576134004</v>
-      </c>
-      <c r="E2">
-        <v>28.3689261290323</v>
-      </c>
-      <c r="F2">
-        <v>58</v>
-      </c>
-      <c r="G2">
-        <v>57.793366666666699</v>
-      </c>
-      <c r="H2">
-        <v>2182.50765</v>
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3">
-        <v>6.6006172693903</v>
+        <v>6.6774736802061101</v>
       </c>
       <c r="D3">
-        <v>5.9308065039859104</v>
+        <v>6.0704386576134004</v>
       </c>
       <c r="E3">
-        <v>31.892729838709698</v>
+        <v>28.3689261290323</v>
       </c>
       <c r="F3">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="G3">
-        <v>93.900033333333297</v>
+        <v>57.793366666666699</v>
       </c>
       <c r="H3">
-        <v>2201.75043333333</v>
+        <v>2182.50765</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4">
-        <v>7.7522940891021896</v>
+        <v>6.6006172693903</v>
       </c>
       <c r="D4">
-        <v>9.1622820249045294</v>
+        <v>5.9308065039859104</v>
       </c>
       <c r="E4">
-        <v>34.161196699129</v>
+        <v>31.892729838709698</v>
       </c>
       <c r="F4">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="G4">
-        <v>29.954266621166699</v>
+        <v>93.900033333333297</v>
       </c>
       <c r="H4">
-        <v>2426.4740505448299</v>
+        <v>2201.75043333333</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5">
-        <v>8.5361044298057607</v>
+        <v>7.7522940891021896</v>
       </c>
       <c r="D5">
-        <v>8.6778669421049806</v>
+        <v>9.1622820249045294</v>
       </c>
       <c r="E5">
-        <v>29.849193548387099</v>
+        <v>34.161196699129</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="G5">
-        <v>11.0833333333333</v>
+        <v>29.954266621166699</v>
       </c>
       <c r="H5">
-        <v>2380.3404761904799</v>
+        <v>2426.4740505448299</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -640,25 +639,25 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6">
-        <v>7.3846573353108402</v>
+        <v>8.5361044298057607</v>
       </c>
       <c r="D6">
-        <v>10.1731973717791</v>
+        <v>8.6778669421049806</v>
       </c>
       <c r="E6">
-        <v>40.320161290322602</v>
+        <v>29.849193548387099</v>
       </c>
       <c r="F6">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>12.75</v>
+        <v>11.0833333333333</v>
       </c>
       <c r="H6">
-        <v>2078.2023809523798</v>
+        <v>2380.3404761904799</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -666,25 +665,25 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7">
-        <v>6.5036492567499202</v>
+        <v>7.3846573353108402</v>
       </c>
       <c r="D7">
-        <v>4.5187893956247702</v>
+        <v>10.1731973717791</v>
       </c>
       <c r="E7">
-        <v>26.187096774193499</v>
+        <v>40.320161290322602</v>
       </c>
       <c r="F7">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="G7">
-        <v>8.5</v>
+        <v>12.75</v>
       </c>
       <c r="H7">
-        <v>1833.3333333333301</v>
+        <v>2078.2023809523798</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -692,25 +691,25 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8">
-        <v>6.5124966091873802</v>
+        <v>6.5036492567499202</v>
       </c>
       <c r="D8">
-        <v>6.26662597691519</v>
+        <v>4.5187893956247702</v>
       </c>
       <c r="E8">
-        <v>28.306451612903199</v>
+        <v>26.187096774193499</v>
       </c>
       <c r="F8">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="G8">
-        <v>1.5833333333333299</v>
+        <v>8.5</v>
       </c>
       <c r="H8">
-        <v>1775.8333333333301</v>
+        <v>1833.3333333333301</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -718,51 +717,51 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9">
-        <v>6.7464966685767598</v>
+        <v>6.5124966091873802</v>
       </c>
       <c r="D9">
-        <v>6.9997996812234904</v>
+        <v>6.26662597691519</v>
       </c>
       <c r="E9">
-        <v>28.367857142857101</v>
+        <v>28.306451612903199</v>
       </c>
       <c r="F9">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>1.5833333333333299</v>
       </c>
       <c r="H9">
-        <v>1860.2142857142901</v>
+        <v>1775.8333333333301</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C10">
-        <v>6.6009699977441896</v>
+        <v>6.7464966685767598</v>
       </c>
       <c r="D10">
-        <v>5.3096153846153804</v>
+        <v>6.9997996812234904</v>
       </c>
       <c r="E10">
-        <v>25.557692307692299</v>
+        <v>28.367857142857101</v>
       </c>
       <c r="F10">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G10">
-        <v>12.1666666666667</v>
+        <v>0</v>
       </c>
       <c r="H10">
-        <v>1975.5952380952399</v>
+        <v>1860.2142857142901</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -770,25 +769,25 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11">
-        <v>7.9841290877581201</v>
+        <v>6.6009699977441896</v>
       </c>
       <c r="D11">
-        <v>7.5570821651466797</v>
+        <v>5.3096153846153804</v>
       </c>
       <c r="E11">
-        <v>31.258064516129</v>
+        <v>25.557692307692299</v>
       </c>
       <c r="F11">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="G11">
-        <v>4.1666666666666696</v>
+        <v>12.1666666666667</v>
       </c>
       <c r="H11">
-        <v>2341.5261904761901</v>
+        <v>1975.5952380952399</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -796,51 +795,51 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12">
-        <v>4.8270882343463004</v>
+        <v>7.9841290877581201</v>
       </c>
       <c r="D12">
-        <v>2.6932121641799101</v>
+        <v>7.5570821651466797</v>
       </c>
       <c r="E12">
-        <v>16.903225806451601</v>
+        <v>31.258064516129</v>
       </c>
       <c r="F12">
-        <v>56</v>
+        <v>6</v>
       </c>
       <c r="G12">
-        <v>5</v>
+        <v>4.1666666666666696</v>
       </c>
       <c r="H12">
-        <v>1375.2738095238101</v>
+        <v>2341.5261904761901</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13">
-        <v>7.8799300208504901</v>
+        <v>4.8270882343463004</v>
       </c>
       <c r="D13">
-        <v>6.1421467575805702</v>
+        <v>2.6932121641799101</v>
       </c>
       <c r="E13">
-        <v>28.2258064516129</v>
+        <v>16.903225806451601</v>
       </c>
       <c r="F13">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H13">
-        <v>2190.8523809523799</v>
+        <v>1375.2738095238101</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -848,51 +847,51 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14">
-        <v>7.7343277443110603</v>
+        <v>7.8799300208504901</v>
       </c>
       <c r="D14">
-        <v>7.8939708141320999</v>
+        <v>6.1421467575805702</v>
       </c>
       <c r="E14">
-        <v>33.1782258064516</v>
+        <v>28.2258064516129</v>
       </c>
       <c r="F14">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="G14">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="H14">
-        <v>2190.2857142857101</v>
+        <v>2190.8523809523799</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15">
-        <v>6.8401662853275802</v>
+        <v>7.7343277443110603</v>
       </c>
       <c r="D15">
-        <v>5.2736666559247203</v>
+        <v>7.8939708141320999</v>
       </c>
       <c r="E15">
-        <v>23.903225806451601</v>
+        <v>33.1782258064516</v>
       </c>
       <c r="F15">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="G15">
-        <v>3.75</v>
+        <v>4.5</v>
       </c>
       <c r="H15">
-        <v>1951.94047619048</v>
+        <v>2190.2857142857101</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -900,25 +899,25 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16">
-        <v>6.3902585765489004</v>
+        <v>6.8401662853275802</v>
       </c>
       <c r="D16">
-        <v>6.6765659072110699</v>
+        <v>5.2736666559247203</v>
       </c>
       <c r="E16">
-        <v>28.951612903225801</v>
+        <v>23.903225806451601</v>
       </c>
       <c r="F16">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="G16">
-        <v>7</v>
+        <v>3.75</v>
       </c>
       <c r="H16">
-        <v>1896.9047619047601</v>
+        <v>1951.94047619048</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -926,25 +925,25 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17">
-        <v>5.5095888430565898</v>
+        <v>6.3902585765489004</v>
       </c>
       <c r="D17">
-        <v>4.51065977033719</v>
+        <v>6.6765659072110699</v>
       </c>
       <c r="E17">
-        <v>22.693548387096801</v>
+        <v>28.951612903225801</v>
       </c>
       <c r="F17">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="G17">
-        <v>8.4166666666666696</v>
+        <v>7</v>
       </c>
       <c r="H17">
-        <v>1595.75</v>
+        <v>1896.9047619047601</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -952,28 +951,70 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18">
+        <v>5.5095888430565898</v>
+      </c>
+      <c r="D18">
+        <v>4.51065977033719</v>
+      </c>
+      <c r="E18">
+        <v>22.693548387096801</v>
+      </c>
+      <c r="F18">
+        <v>8</v>
+      </c>
+      <c r="G18">
+        <v>8.4166666666666696</v>
+      </c>
+      <c r="H18">
+        <v>1595.75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" t="s">
         <v>29</v>
       </c>
-      <c r="C18">
+      <c r="C19">
         <v>6.4650021125827601</v>
       </c>
-      <c r="D18">
+      <c r="D19">
         <v>7.5087788555530501</v>
       </c>
-      <c r="E18">
+      <c r="E19">
         <v>27.951612903225801</v>
       </c>
-      <c r="F18">
+      <c r="F19">
         <v>16</v>
       </c>
-      <c r="G18">
+      <c r="G19">
         <v>6.25</v>
       </c>
-      <c r="H18">
+      <c r="H19">
         <v>1869.4642857142901</v>
       </c>
     </row>
+    <row r="20" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A20:H20"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>